<commit_message>
Writing of retest results in Excel file done
</commit_message>
<xml_diff>
--- a/src/test/resources/Reports/Verification.xlsx
+++ b/src/test/resources/Reports/Verification.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40C02820-BA6E-4176-ACD0-D59D9B70E49D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="795" windowWidth="23250" windowHeight="12720"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,14 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="41">
   <si>
     <t>Numero bug</t>
   </si>
   <si>
-    <t>Satut Bug</t>
-  </si>
-  <si>
     <t>Date Verification</t>
   </si>
   <si>
@@ -35,12 +31,124 @@
   </si>
   <si>
     <t>LEROY MERLIN</t>
+  </si>
+  <si>
+    <t>KO</t>
+  </si>
+  <si>
+    <t>2021-07-12</t>
+  </si>
+  <si>
+    <t>1024</t>
+  </si>
+  <si>
+    <t>14:07:16</t>
+  </si>
+  <si>
+    <t>997</t>
+  </si>
+  <si>
+    <t>14:08:06</t>
+  </si>
+  <si>
+    <t>1011</t>
+  </si>
+  <si>
+    <t>14:10:32</t>
+  </si>
+  <si>
+    <t>Statut Bug</t>
+  </si>
+  <si>
+    <t>14:34:12</t>
+  </si>
+  <si>
+    <t>14:35:30</t>
+  </si>
+  <si>
+    <t>14:36:16</t>
+  </si>
+  <si>
+    <t>14:37:08</t>
+  </si>
+  <si>
+    <t>14:37:54</t>
+  </si>
+  <si>
+    <t>14:40:26</t>
+  </si>
+  <si>
+    <t>14:41:12</t>
+  </si>
+  <si>
+    <t>14:41:58</t>
+  </si>
+  <si>
+    <t>14:42:46</t>
+  </si>
+  <si>
+    <t>14:43:32</t>
+  </si>
+  <si>
+    <t>15:15:46</t>
+  </si>
+  <si>
+    <t>15:16:39</t>
+  </si>
+  <si>
+    <t>15:17:27</t>
+  </si>
+  <si>
+    <t>16:17:15</t>
+  </si>
+  <si>
+    <t>16:18:10</t>
+  </si>
+  <si>
+    <t>16:19:00</t>
+  </si>
+  <si>
+    <t>16:22:16</t>
+  </si>
+  <si>
+    <t>16:22:41</t>
+  </si>
+  <si>
+    <t>16:23:26</t>
+  </si>
+  <si>
+    <t>16:24:13</t>
+  </si>
+  <si>
+    <t>16:25:00</t>
+  </si>
+  <si>
+    <t>16:25:47</t>
+  </si>
+  <si>
+    <t>16:25:48</t>
+  </si>
+  <si>
+    <t>16:54:18</t>
+  </si>
+  <si>
+    <t>16:54:45</t>
+  </si>
+  <si>
+    <t>16:55:27</t>
+  </si>
+  <si>
+    <t>16:55:52</t>
+  </si>
+  <si>
+    <t>16:56:19</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -476,47 +584,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="185" zoomScaleNormal="176" zoomScalePageLayoutView="185" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A3" zoomScale="185" zoomScaleNormal="176" zoomScalePageLayoutView="185" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="8"/>
     </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" hidden="1">
@@ -548,6 +656,48 @@
     </row>
     <row r="13" spans="1:4" hidden="1">
       <c r="B13" s="2"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Test listener class added
</commit_message>
<xml_diff>
--- a/src/test/resources/Reports/Verification.xlsx
+++ b/src/test/resources/Reports/Verification.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="45">
   <si>
     <t>Numero bug</t>
   </si>
@@ -142,6 +142,18 @@
   </si>
   <si>
     <t>16:56:19</t>
+  </si>
+  <si>
+    <t>2021-07-13</t>
+  </si>
+  <si>
+    <t>16:06:37</t>
+  </si>
+  <si>
+    <t>16:07:33</t>
+  </si>
+  <si>
+    <t>16:08:18</t>
   </si>
 </sst>
 </file>
@@ -665,10 +677,10 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15">
@@ -679,10 +691,10 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16">

</xml_diff>